<commit_message>
Revised getCoralName. Added tostring on coral info. Added two new types of test (Random)
</commit_message>
<xml_diff>
--- a/Coral Chart.xlsx
+++ b/Coral Chart.xlsx
@@ -85,7 +85,7 @@
     <t>soilPreference8</t>
   </si>
   <si>
-    <t>preference9</t>
+    <t>coralPreference9</t>
   </si>
   <si>
     <r>
@@ -897,7 +897,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -912,7 +912,7 @@
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.0255102040816"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.3979591836735"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.5714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.2857142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.9642857142857"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.6734693877551"/>
   </cols>
   <sheetData>

</xml_diff>